<commit_message>
Added new Cape of Umbar deed
</commit_message>
<xml_diff>
--- a/SourceFiles/DeedInfo-10-Haradwaith.xlsx
+++ b/SourceFiles/DeedInfo-10-Haradwaith.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkckx\Documents\The Lord of the Rings Online\Plugins\CubePlugins\DeedTracker\SourceFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627DBA7B-31BF-4CAF-89F1-D6E5DAA20A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4152E3B6-5F06-46E4-9D2C-694037B037CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="465" windowWidth="24435" windowHeight="14865" tabRatio="869" activeTab="7" xr2:uid="{CDC9C16A-58F0-4807-B5CD-F77FF9D2EA43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="869" activeTab="6" xr2:uid="{CDC9C16A-58F0-4807-B5CD-F77FF9D2EA43}"/>
   </bookViews>
   <sheets>
     <sheet name="Type" sheetId="2" r:id="rId1"/>
@@ -544,12 +544,6 @@
     <t>Great Aspirations - Demand</t>
   </si>
   <si>
-    <t>Haradrim-slayer of the Cape of Umbar (Advanced)</t>
-  </si>
-  <si>
-    <t>Haradrim-slayer of the Cape of Umbar</t>
-  </si>
-  <si>
     <t>Deeds of Umbar Baharbêl</t>
   </si>
   <si>
@@ -602,6 +596,12 @@
   </si>
   <si>
     <t>Umbar Completionist</t>
+  </si>
+  <si>
+    <t>The Depths of Mâkhda Khorbo -- Azagath's Escape</t>
+  </si>
+  <si>
+    <t>The Depths of Mâkhda Khorbo</t>
   </si>
 </sst>
 </file>
@@ -657,9 +657,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -697,7 +697,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -803,7 +803,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -945,7 +945,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3112,10 +3112,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CF1D9D-0842-4870-8161-749AA38F3E6F}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F2:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3212,31 +3212,31 @@
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F27" si="0">CONCATENATE(H3,I3,J3,L3," -- ",B3)</f>
+        <f t="shared" ref="F3:F28" si="0">CONCATENATE(H3,I3,J3,L3," -- ",B3)</f>
         <v xml:space="preserve"> [2] = {["ID"] = 1879474829; }; -- Explorer of the Cape of Umbar</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G27" si="1">ROW()-1</f>
+        <f t="shared" ref="G3:G28" si="1">ROW()-1</f>
         <v>2</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H32" si="2">CONCATENATE(REPT(" ",2-LEN(G3)),"[",G3,"] = {")</f>
+        <f t="shared" ref="H3:H33" si="2">CONCATENATE(REPT(" ",2-LEN(G3)),"[",G3,"] = {")</f>
         <v xml:space="preserve"> [2] = {</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I32" si="3">IF(LEN(A3)&gt;0,CONCATENATE("[""ID""] = ",A3,"; "),"")</f>
+        <f t="shared" ref="I3:I33" si="3">IF(LEN(A3)&gt;0,CONCATENATE("[""ID""] = ",A3,"; "),"")</f>
         <v xml:space="preserve">["ID"] = 1879474829; </v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J32" si="4">IF(LEN(D3)&gt;0,CONCATENATE("[""CAT_ID""] = ",D3,"; "),"")</f>
+        <f t="shared" ref="J3:J33" si="4">IF(LEN(D3)&gt;0,CONCATENATE("[""CAT_ID""] = ",D3,"; "),"")</f>
         <v/>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K32" si="5">CONCATENATE("[""TIER""] = ",TEXT(C3,"0"),"; ")</f>
+        <f t="shared" ref="K3:K33" si="5">CONCATENATE("[""TIER""] = ",TEXT(C3,"0"),"; ")</f>
         <v xml:space="preserve">["TIER"] = 1; </v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L32" si="6">CONCATENATE("};")</f>
+        <f t="shared" ref="L3:L33" si="6">CONCATENATE("};")</f>
         <v>};</v>
       </c>
     </row>
@@ -3982,37 +3982,34 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1879474824</v>
-      </c>
       <c r="B23" t="s">
-        <v>167</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
+        <v>186</v>
+      </c>
+      <c r="D23">
+        <v>299</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v>[22] = {["ID"] = 1879474824; }; -- Haradrim-slayer of the Cape of Umbar (Advanced)</v>
+        <f t="shared" ref="F23:F27" si="7">CONCATENATE(H23,I23,J23,L23," -- ",B23)</f>
+        <v>[22] = {["CAT_ID"] = 299; }; -- The Depths of Mâkhda Khorbo</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="H23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H23:H27" si="8">CONCATENATE(REPT(" ",2-LEN(G23)),"[",G23,"] = {")</f>
         <v>[22] = {</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">["ID"] = 1879474824; </v>
+        <f t="shared" ref="I23:I27" si="9">IF(LEN(A23)&gt;0,CONCATENATE("[""ID""] = ",A23,"; "),"")</f>
+        <v/>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ref="J23:J27" si="10">IF(LEN(D23)&gt;0,CONCATENATE("[""CAT_ID""] = ",D23,"; "),"")</f>
+        <v xml:space="preserve">["CAT_ID"] = 299; </v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="K23:K27" si="11">CONCATENATE("[""TIER""] = ",TEXT(C23,"0"),"; ")</f>
         <v xml:space="preserve">["TIER"] = 0; </v>
       </c>
       <c r="L23" t="str">
@@ -4022,37 +4019,37 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>1879474820</v>
+        <v>1879482825</v>
       </c>
       <c r="B24" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="0"/>
-        <v>[23] = {["ID"] = 1879474820; }; -- Haradrim-slayer of the Cape of Umbar</v>
+        <f t="shared" si="7"/>
+        <v>[23] = {["ID"] = 1879482825; }; -- The Depths of Mâkhda Khorbo -- Azagath's Escape</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>[23] = {</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">["ID"] = 1879474820; </v>
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">["ID"] = 1879482825; </v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 1; </v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="6"/>
@@ -4061,7 +4058,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">[24] = {}; -- </v>
       </c>
       <c r="G25">
@@ -4069,19 +4066,19 @@
         <v>24</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>[24] = {</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">["TIER"] = 0; </v>
       </c>
       <c r="L25" t="str">
@@ -4091,7 +4088,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">[25] = {}; -- </v>
       </c>
       <c r="G26">
@@ -4099,19 +4096,19 @@
         <v>25</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>[25] = {</v>
       </c>
       <c r="I26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="J26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">["TIER"] = 0; </v>
       </c>
       <c r="L26" t="str">
@@ -4121,7 +4118,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">[26] = {}; -- </v>
       </c>
       <c r="G27">
@@ -4129,19 +4126,19 @@
         <v>26</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>[26] = {</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">["TIER"] = 0; </v>
       </c>
       <c r="L27" t="str">
@@ -4150,9 +4147,17 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[27] = {}; -- </v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
       <c r="H28" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">  [] = {</v>
+        <v>[27] = {</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="3"/>
@@ -4255,6 +4260,28 @@
         <v xml:space="preserve">["TIER"] = 0; </v>
       </c>
       <c r="L32" t="str">
+        <f t="shared" si="6"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="33" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H33" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  [] = {</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="L33" t="str">
         <f t="shared" si="6"/>
         <v>};</v>
       </c>
@@ -4269,7 +4296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E20F2D1-5B1C-4EE5-AF25-70FDE67F21F0}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -4322,7 +4349,7 @@
         <v>1879477448</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -4361,7 +4388,7 @@
         <v>1879477540</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -4400,7 +4427,7 @@
         <v>1879477537</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -4439,7 +4466,7 @@
         <v>1879477538</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -4478,7 +4505,7 @@
         <v>1879477539</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -4517,7 +4544,7 @@
         <v>1879477767</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -4556,7 +4583,7 @@
         <v>1879477633</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -4595,7 +4622,7 @@
         <v>1879477653</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -4634,7 +4661,7 @@
         <v>1879477652</v>
       </c>
       <c r="B10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -4673,7 +4700,7 @@
         <v>1879477650</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -4712,7 +4739,7 @@
         <v>1879477654</v>
       </c>
       <c r="B12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -4751,7 +4778,7 @@
         <v>1879477651</v>
       </c>
       <c r="B13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -4790,7 +4817,7 @@
         <v>1879477840</v>
       </c>
       <c r="B14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -4829,7 +4856,7 @@
         <v>1879477769</v>
       </c>
       <c r="B15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -4868,7 +4895,7 @@
         <v>1879477768</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -4907,7 +4934,7 @@
         <v>1879477838</v>
       </c>
       <c r="B17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -4946,7 +4973,7 @@
         <v>1879477839</v>
       </c>
       <c r="B18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -4985,7 +5012,7 @@
         <v>1879478542</v>
       </c>
       <c r="B19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C19">
         <v>0</v>

</xml_diff>

<commit_message>
Added U40 Umbar Baharbêl deeds
</commit_message>
<xml_diff>
--- a/SourceFiles/DeedInfo-10-Haradwaith.xlsx
+++ b/SourceFiles/DeedInfo-10-Haradwaith.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkckx\Documents\The Lord of the Rings Online\Plugins\CubePlugins\DeedTracker\SourceFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4152E3B6-5F06-46E4-9D2C-694037B037CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B126BDF-C106-4370-9437-8771C1B696FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="869" activeTab="6" xr2:uid="{CDC9C16A-58F0-4807-B5CD-F77FF9D2EA43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="869" activeTab="7" xr2:uid="{CDC9C16A-58F0-4807-B5CD-F77FF9D2EA43}"/>
   </bookViews>
   <sheets>
     <sheet name="Type" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="283">
   <si>
     <t>TIER</t>
   </si>
@@ -602,14 +602,310 @@
   </si>
   <si>
     <t>The Depths of Mâkhda Khorbo</t>
+  </si>
+  <si>
+    <t>Light in the Umbar-môkh</t>
+  </si>
+  <si>
+    <t>Tier code</t>
+  </si>
+  <si>
+    <t>Slayer of the Umbar-môkh</t>
+  </si>
+  <si>
+    <t>Slayer of Khabârkhad</t>
+  </si>
+  <si>
+    <t>Crypt-raider Slayer of Khabârkhad (Advanced)</t>
+  </si>
+  <si>
+    <t>Crypt-raider Slayer of Khabârkhad</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Defeat 50 crypt-raiders in Khabârkhad</t>
+  </si>
+  <si>
+    <t>Defeat 100 crypt-raiders in Khabârkhad</t>
+  </si>
+  <si>
+    <t>Spider-bane of Khabârkhad (Advanced)</t>
+  </si>
+  <si>
+    <t>Defeat 100 spiders in Khabârkhad</t>
+  </si>
+  <si>
+    <t>Spider-bane of Khabârkhad</t>
+  </si>
+  <si>
+    <t>Defeat 50 spiders in Khabârkhad</t>
+  </si>
+  <si>
+    <t>Dead-slayer of Khabârkhad (Advanced)</t>
+  </si>
+  <si>
+    <t>Dead-slayer of Khabârkhad</t>
+  </si>
+  <si>
+    <t>Defeat 50 Dead in Khabârkhad</t>
+  </si>
+  <si>
+    <t>Defeat 100 Dead in Khabârkhad</t>
+  </si>
+  <si>
+    <t>Slayer of Ilmabiri</t>
+  </si>
+  <si>
+    <t>Forsaken-slayer of Ilmabiri (Advanced)</t>
+  </si>
+  <si>
+    <t>Forsaken-slayer of Ilmabiri</t>
+  </si>
+  <si>
+    <t>Defeat 50 forsaken in Ilmabiri</t>
+  </si>
+  <si>
+    <t>Defeat 100 forsaken in Ilmabiri</t>
+  </si>
+  <si>
+    <t>Goblin-slayer of Ilmabiri (Advanced)</t>
+  </si>
+  <si>
+    <t>Goblin-slayer of Ilmabiri</t>
+  </si>
+  <si>
+    <t>Defeat 50 goblins in Ilmabiri</t>
+  </si>
+  <si>
+    <t>Defeat 100 goblins in Ilmabiri</t>
+  </si>
+  <si>
+    <t>Crocodile-slayer of Ilmabiri (Advanced)</t>
+  </si>
+  <si>
+    <t>Crocodile-slayer of Ilmabiri</t>
+  </si>
+  <si>
+    <t>Defeat 25 crocodiles in Ilmabiri</t>
+  </si>
+  <si>
+    <t>Defeat 75 crocodiles in Ilmabiri</t>
+  </si>
+  <si>
+    <t>Slayer of Kamrabezûr</t>
+  </si>
+  <si>
+    <t>Cultist-slayer of Kamrabezûr (Advanced)</t>
+  </si>
+  <si>
+    <t>Cultist-slayer of Kamrabezûr</t>
+  </si>
+  <si>
+    <t>Defeat 50 cultists in Kamrabezûr</t>
+  </si>
+  <si>
+    <t>Defeat 100 cultists in Kamrabezûr</t>
+  </si>
+  <si>
+    <t>Gladiator-slayer of Kamrabezûr (Advanced)</t>
+  </si>
+  <si>
+    <t>Gladiator-slayer of Kamrabezûr</t>
+  </si>
+  <si>
+    <t>Defeat 50 gladiators in Kamrabezûr</t>
+  </si>
+  <si>
+    <t>Defeat 100 gladiators in Kamrabezûr</t>
+  </si>
+  <si>
+    <t>Dead-slayer of Kamrabezûr (Advanced)</t>
+  </si>
+  <si>
+    <t>Dead-slayer of Kamrabezûr</t>
+  </si>
+  <si>
+    <t>Defeat 50 Dead in Kamrabezûr</t>
+  </si>
+  <si>
+    <t>Defeat 100 Dead in Kamrabezûr</t>
+  </si>
+  <si>
+    <t>Slayer of Tâkhdar</t>
+  </si>
+  <si>
+    <t>Grodbog-slayer of Tâkhdar (Advanced)</t>
+  </si>
+  <si>
+    <t>Grodbog-slayer of Tâkhdar</t>
+  </si>
+  <si>
+    <t>Defeat 50 gredbyg in Tâkhdar</t>
+  </si>
+  <si>
+    <t>Defeat 100 gredbyg in Tâkhdar</t>
+  </si>
+  <si>
+    <t>Smuggler-bane of Tâkhdar (Advanced)</t>
+  </si>
+  <si>
+    <t>Smuggler-bane of Tâkhdar</t>
+  </si>
+  <si>
+    <t>Defeat 50 smugglers in Tâkhdar</t>
+  </si>
+  <si>
+    <t>Defeat 100 smugglers in Tâkhdar</t>
+  </si>
+  <si>
+    <t>Spider-bane of Tâkhdar (Advanced)</t>
+  </si>
+  <si>
+    <t>Defeat 50 spiders in Tâkhdar</t>
+  </si>
+  <si>
+    <t>Defeat 100 spiders in Tâkhdar</t>
+  </si>
+  <si>
+    <t>Spider-bane of Tâkhdar</t>
+  </si>
+  <si>
+    <t>Slayer of Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Smuggler-bane of Dil-irmíz (Advanced)</t>
+  </si>
+  <si>
+    <t>Smuggler-bane of Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Defeat 50 smugglers in Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Defeat 75 smugglers in Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Criminal-bane of Dil-irmíz (Advanced)</t>
+  </si>
+  <si>
+    <t>Criminal-bane of Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Defeat 50 criminals in Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Defeat 75 criminals in Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Umbar-môkh</t>
+  </si>
+  <si>
+    <t>Explorer of the Umbar-môkh</t>
+  </si>
+  <si>
+    <t>Reclaiming Khabârkhad</t>
+  </si>
+  <si>
+    <t>Reclaiming Ilmabiri</t>
+  </si>
+  <si>
+    <t>Reclaiming Kamrabezûr</t>
+  </si>
+  <si>
+    <t>Reclaiming Tâkhdar</t>
+  </si>
+  <si>
+    <t>Reclaiming Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Tales of the Umbar-môkh</t>
+  </si>
+  <si>
+    <t>Tales of Khabârkhad</t>
+  </si>
+  <si>
+    <t>Tales of Ilmabiri</t>
+  </si>
+  <si>
+    <t>Tales of Kamrabezûr</t>
+  </si>
+  <si>
+    <t>Tales of Tâkhdar</t>
+  </si>
+  <si>
+    <t>Tales of Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Vanquisher of Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Cultist-bane of Dil-irmíz (Advanced)</t>
+  </si>
+  <si>
+    <t>Defeat 100 Umshûran cultists in Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Cultist-bane of Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Defeat 50 Umshûran cultists in Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Darkwater-slayer of Dil-irmíz (Advanced)</t>
+  </si>
+  <si>
+    <t>Darkwater-slayer of Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Defeat 50 darkwaters in Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Defeat 100 darkwaters in Dil-irmíz</t>
+  </si>
+  <si>
+    <t>Rat-slayer of the Umbar-môkh (Advanced)</t>
+  </si>
+  <si>
+    <t>Rat-slayer of the Umbar-môkh</t>
+  </si>
+  <si>
+    <t>Defeat 100 rats in the Umbar-môkh</t>
+  </si>
+  <si>
+    <t>Defeat 200 rats in the Umbar-môkh</t>
+  </si>
+  <si>
+    <t>Bat-slayer of the Umbar-môkh (Advanced)</t>
+  </si>
+  <si>
+    <t>Bat-slayer of the Umbar-môkh</t>
+  </si>
+  <si>
+    <t>Defeat 100 bats in the Umbar-môkh</t>
+  </si>
+  <si>
+    <t>Defeat 200 bats in the Umbar-môkh</t>
+  </si>
+  <si>
+    <t>Treasure-seeker of the Umbar-môkh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -637,8 +933,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3114,7 +3411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CF1D9D-0842-4870-8161-749AA38F3E6F}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F2:F24"/>
     </sheetView>
   </sheetViews>
@@ -4294,10 +4591,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E20F2D1-5B1C-4EE5-AF25-70FDE67F21F0}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4305,11 +4605,11 @@
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="48.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="85.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="85.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>121</v>
       </c>
@@ -4322,29 +4622,35 @@
       <c r="D1" t="s">
         <v>122</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1" t="s">
         <v>124</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>125</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>123</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>122</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>126</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1879477448</v>
       </c>
@@ -4354,36 +4660,40 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="F2" t="str">
-        <f>CONCATENATE(H2,I2,J2,L2," -- ",B2)</f>
+      <c r="G2" t="str">
+        <f>IF(AND(A2&gt;0,C2&gt;0),CONCATENATE("[",A2,"] = ",C2,", // ",B2),"")</f>
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <f>CONCATENATE(J2,K2,L2,N2," -- ",B2)</f>
         <v xml:space="preserve"> [1] = {["ID"] = 1879477448; }; -- Deeds of Umbar Baharbêl</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="H2" t="str">
-        <f>CONCATENATE(REPT(" ",2-LEN(G2)),"[",G2,"] = {")</f>
+      <c r="J2" t="str">
+        <f>CONCATENATE(REPT(" ",2-LEN(I2)),"[",I2,"] = {")</f>
         <v xml:space="preserve"> [1] = {</v>
       </c>
-      <c r="I2" t="str">
+      <c r="K2" t="str">
         <f>IF(LEN(A2)&gt;0,CONCATENATE("[""ID""] = ",A2,"; "),"")</f>
         <v xml:space="preserve">["ID"] = 1879477448; </v>
       </c>
-      <c r="J2" t="str">
+      <c r="L2" t="str">
         <f>IF(LEN(D2)&gt;0,CONCATENATE("[""CAT_ID""] = ",D2,"; "),"")</f>
         <v/>
       </c>
-      <c r="K2" t="str">
+      <c r="M2" t="str">
         <f>CONCATENATE("[""TIER""] = ",TEXT(C2,"0"),"; ")</f>
         <v xml:space="preserve">["TIER"] = 0; </v>
       </c>
-      <c r="L2" t="str">
+      <c r="N2" t="str">
         <f>CONCATENATE("};")</f>
         <v>};</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1879477540</v>
       </c>
@@ -4393,36 +4703,40 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F27" si="0">CONCATENATE(H3,I3,J3,L3," -- ",B3)</f>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G66" si="0">IF(AND(A3&gt;0,C3&gt;0),CONCATENATE("[",A3,"] = ",C3,", // ",B3),"")</f>
+        <v>[1879477540] = 1, // Quests of Umbar Baharbêl</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H66" si="1">CONCATENATE(J3,K3,L3,N3," -- ",B3)</f>
         <v xml:space="preserve"> [2] = {["ID"] = 1879477540; }; -- Quests of Umbar Baharbêl</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G27" si="1">ROW()-1</f>
+      <c r="I3">
+        <f t="shared" ref="I3:I66" si="2">ROW()-1</f>
         <v>2</v>
       </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H32" si="2">CONCATENATE(REPT(" ",2-LEN(G3)),"[",G3,"] = {")</f>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J66" si="3">CONCATENATE(REPT(" ",2-LEN(I3)),"[",I3,"] = {")</f>
         <v xml:space="preserve"> [2] = {</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I32" si="3">IF(LEN(A3)&gt;0,CONCATENATE("[""ID""] = ",A3,"; "),"")</f>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K66" si="4">IF(LEN(A3)&gt;0,CONCATENATE("[""ID""] = ",A3,"; "),"")</f>
         <v xml:space="preserve">["ID"] = 1879477540; </v>
       </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J32" si="4">IF(LEN(D3)&gt;0,CONCATENATE("[""CAT_ID""] = ",D3,"; "),"")</f>
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <f t="shared" ref="K3:K32" si="5">CONCATENATE("[""TIER""] = ",TEXT(C3,"0"),"; ")</f>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L66" si="5">IF(LEN(D3)&gt;0,CONCATENATE("[""CAT_ID""] = ",D3,"; "),"")</f>
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M66" si="6">CONCATENATE("[""TIER""] = ",TEXT(C3,"0"),"; ")</f>
         <v xml:space="preserve">["TIER"] = 1; </v>
       </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L32" si="6">CONCATENATE("};")</f>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N66" si="7">CONCATENATE("};")</f>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1879477537</v>
       </c>
@@ -4432,36 +4746,40 @@
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="F4" t="str">
-        <f t="shared" si="0"/>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477537] = 2, // Tales of the Free City (Final)</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> [3] = {["ID"] = 1879477537; }; -- Tales of the Free City (Final)</v>
       </c>
-      <c r="G4">
-        <f t="shared" si="1"/>
+      <c r="I4">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H4" t="str">
-        <f t="shared" si="2"/>
+      <c r="J4" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> [3] = {</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" si="3"/>
+      <c r="K4" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477537; </v>
       </c>
-      <c r="J4" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K4" t="str">
-        <f t="shared" si="5"/>
+      <c r="L4" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
-      <c r="L4" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1879477538</v>
       </c>
@@ -4471,36 +4789,40 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477538] = 2, // Tales of the Free City (Advanced)</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> [4] = {["ID"] = 1879477538; }; -- Tales of the Free City (Advanced)</v>
       </c>
-      <c r="G5">
-        <f t="shared" si="1"/>
+      <c r="I5">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="H5" t="str">
-        <f t="shared" si="2"/>
+      <c r="J5" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> [4] = {</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="3"/>
+      <c r="K5" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477538; </v>
       </c>
-      <c r="J5" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K5" t="str">
-        <f t="shared" si="5"/>
+      <c r="L5" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
-      <c r="L5" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1879477539</v>
       </c>
@@ -4510,36 +4832,40 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477539] = 2, // Tales of the Free City</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> [5] = {["ID"] = 1879477539; }; -- Tales of the Free City</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="1"/>
+      <c r="I6">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H6" t="str">
-        <f t="shared" si="2"/>
+      <c r="J6" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> [5] = {</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="3"/>
+      <c r="K6" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477539; </v>
       </c>
-      <c r="J6" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K6" t="str">
-        <f t="shared" si="5"/>
+      <c r="L6" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
-      <c r="L6" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1879477767</v>
       </c>
@@ -4549,36 +4875,40 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477767] = 1, // Explorer of Umbar Baharbêl</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> [6] = {["ID"] = 1879477767; }; -- Explorer of Umbar Baharbêl</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="1"/>
+      <c r="I7">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="H7" t="str">
-        <f t="shared" si="2"/>
+      <c r="J7" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> [6] = {</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="3"/>
+      <c r="K7" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477767; </v>
       </c>
-      <c r="J7" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="5"/>
+      <c r="L7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 1; </v>
       </c>
-      <c r="L7" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N7" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1879477633</v>
       </c>
@@ -4588,36 +4918,40 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477633] = 2, // Umbar Baharbêl, the City of the Corsairs</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> [7] = {["ID"] = 1879477633; }; -- Umbar Baharbêl, the City of the Corsairs</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="1"/>
+      <c r="I8">
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="H8" t="str">
-        <f t="shared" si="2"/>
+      <c r="J8" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> [7] = {</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="3"/>
+      <c r="K8" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477633; </v>
       </c>
-      <c r="J8" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K8" t="str">
-        <f t="shared" si="5"/>
+      <c r="L8" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
-      <c r="L8" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1879477653</v>
       </c>
@@ -4627,36 +4961,40 @@
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477653] = 2, // The Gates of Umbar Baharbêl</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> [8] = {["ID"] = 1879477653; }; -- The Gates of Umbar Baharbêl</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="1"/>
+      <c r="I9">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="H9" t="str">
-        <f t="shared" si="2"/>
+      <c r="J9" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> [8] = {</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="3"/>
+      <c r="K9" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477653; </v>
       </c>
-      <c r="J9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K9" t="str">
-        <f t="shared" si="5"/>
+      <c r="L9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
-      <c r="L9" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1879477652</v>
       </c>
@@ -4666,36 +5004,40 @@
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477652] = 2, // The Guilds of Umbar Baharbêl</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> [9] = {["ID"] = 1879477652; }; -- The Guilds of Umbar Baharbêl</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="1"/>
+      <c r="I10">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="H10" t="str">
-        <f t="shared" si="2"/>
+      <c r="J10" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> [9] = {</v>
       </c>
-      <c r="I10" t="str">
-        <f t="shared" si="3"/>
+      <c r="K10" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477652; </v>
       </c>
-      <c r="J10" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K10" t="str">
-        <f t="shared" si="5"/>
+      <c r="L10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
-      <c r="L10" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1879477650</v>
       </c>
@@ -4705,36 +5047,40 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477650] = 2, // The Markets of Umbar Baharbêl</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
         <v>[10] = {["ID"] = 1879477650; }; -- The Markets of Umbar Baharbêl</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="1"/>
+      <c r="I11">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="H11" t="str">
-        <f t="shared" si="2"/>
+      <c r="J11" t="str">
+        <f t="shared" si="3"/>
         <v>[10] = {</v>
       </c>
-      <c r="I11" t="str">
-        <f t="shared" si="3"/>
+      <c r="K11" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477650; </v>
       </c>
-      <c r="J11" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K11" t="str">
-        <f t="shared" si="5"/>
+      <c r="L11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
-      <c r="L11" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N11" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1879477654</v>
       </c>
@@ -4744,36 +5090,40 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477654] = 2, // The Havens of Umbar Baharbêl</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
         <v>[11] = {["ID"] = 1879477654; }; -- The Havens of Umbar Baharbêl</v>
       </c>
-      <c r="G12">
-        <f t="shared" si="1"/>
+      <c r="I12">
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="H12" t="str">
-        <f t="shared" si="2"/>
+      <c r="J12" t="str">
+        <f t="shared" si="3"/>
         <v>[11] = {</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" si="3"/>
+      <c r="K12" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477654; </v>
       </c>
-      <c r="J12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="5"/>
+      <c r="L12" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
-      <c r="L12" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N12" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1879477651</v>
       </c>
@@ -4783,36 +5133,40 @@
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477651] = 2, // The False Church of Ordâkh</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
         <v>[12] = {["ID"] = 1879477651; }; -- The False Church of Ordâkh</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="1"/>
+      <c r="I13">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="H13" t="str">
-        <f t="shared" si="2"/>
+      <c r="J13" t="str">
+        <f t="shared" si="3"/>
         <v>[12] = {</v>
       </c>
-      <c r="I13" t="str">
-        <f t="shared" si="3"/>
+      <c r="K13" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477651; </v>
       </c>
-      <c r="J13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K13" t="str">
-        <f t="shared" si="5"/>
+      <c r="L13" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
-      <c r="L13" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N13" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1879477840</v>
       </c>
@@ -4822,36 +5176,40 @@
       <c r="C14">
         <v>0</v>
       </c>
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
         <v>[13] = {["ID"] = 1879477840; }; -- Defender of Umbar Baharbêl</v>
       </c>
-      <c r="G14">
-        <f t="shared" si="1"/>
+      <c r="I14">
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="H14" t="str">
-        <f t="shared" si="2"/>
+      <c r="J14" t="str">
+        <f t="shared" si="3"/>
         <v>[13] = {</v>
       </c>
-      <c r="I14" t="str">
-        <f t="shared" si="3"/>
+      <c r="K14" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477840; </v>
       </c>
-      <c r="J14" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K14" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
-      </c>
       <c r="L14" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1879477769</v>
       </c>
@@ -4861,36 +5219,40 @@
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477769] = 1, // Heirsworn-slayer of Umbar Baharbêl (Advanced)</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
         <v>[14] = {["ID"] = 1879477769; }; -- Heirsworn-slayer of Umbar Baharbêl (Advanced)</v>
       </c>
-      <c r="G15">
-        <f t="shared" si="1"/>
+      <c r="I15">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="H15" t="str">
-        <f t="shared" si="2"/>
+      <c r="J15" t="str">
+        <f t="shared" si="3"/>
         <v>[14] = {</v>
       </c>
-      <c r="I15" t="str">
-        <f t="shared" si="3"/>
+      <c r="K15" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477769; </v>
       </c>
-      <c r="J15" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K15" t="str">
-        <f t="shared" si="5"/>
+      <c r="L15" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 1; </v>
       </c>
-      <c r="L15" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N15" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1879477768</v>
       </c>
@@ -4900,36 +5262,40 @@
       <c r="C16">
         <v>2</v>
       </c>
-      <c r="F16" t="str">
-        <f t="shared" si="0"/>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477768] = 2, // Heirsworn-slayer of Umbar Baharbêl</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
         <v>[15] = {["ID"] = 1879477768; }; -- Heirsworn-slayer of Umbar Baharbêl</v>
       </c>
-      <c r="G16">
-        <f t="shared" si="1"/>
+      <c r="I16">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="H16" t="str">
-        <f t="shared" si="2"/>
+      <c r="J16" t="str">
+        <f t="shared" si="3"/>
         <v>[15] = {</v>
       </c>
-      <c r="I16" t="str">
-        <f t="shared" si="3"/>
+      <c r="K16" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477768; </v>
       </c>
-      <c r="J16" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K16" t="str">
-        <f t="shared" si="5"/>
+      <c r="L16" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
-      <c r="L16" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N16" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1879477838</v>
       </c>
@@ -4939,36 +5305,40 @@
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="F17" t="str">
-        <f t="shared" si="0"/>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477838] = 1, // Rat-catcher of Umbar Baharbêl (Advanced)</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
         <v>[16] = {["ID"] = 1879477838; }; -- Rat-catcher of Umbar Baharbêl (Advanced)</v>
       </c>
-      <c r="G17">
-        <f t="shared" si="1"/>
+      <c r="I17">
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="H17" t="str">
-        <f t="shared" si="2"/>
+      <c r="J17" t="str">
+        <f t="shared" si="3"/>
         <v>[16] = {</v>
       </c>
-      <c r="I17" t="str">
-        <f t="shared" si="3"/>
+      <c r="K17" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477838; </v>
       </c>
-      <c r="J17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="5"/>
+      <c r="L17" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 1; </v>
       </c>
-      <c r="L17" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N17" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1879477839</v>
       </c>
@@ -4978,36 +5348,40 @@
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>[1879477839] = 2, // Rat-catcher of Umbar Baharbêl</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
         <v>[17] = {["ID"] = 1879477839; }; -- Rat-catcher of Umbar Baharbêl</v>
       </c>
-      <c r="G18">
-        <f t="shared" si="1"/>
+      <c r="I18">
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="H18" t="str">
-        <f t="shared" si="2"/>
+      <c r="J18" t="str">
+        <f t="shared" si="3"/>
         <v>[17] = {</v>
       </c>
-      <c r="I18" t="str">
-        <f t="shared" si="3"/>
+      <c r="K18" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879477839; </v>
       </c>
-      <c r="J18" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K18" t="str">
-        <f t="shared" si="5"/>
+      <c r="L18" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
-      <c r="L18" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N18" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1879478542</v>
       </c>
@@ -5017,382 +5391,2669 @@
       <c r="C19">
         <v>0</v>
       </c>
-      <c r="F19" t="str">
-        <f t="shared" si="0"/>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
         <v>[18] = {["ID"] = 1879478542; }; -- Umbar Completionist</v>
       </c>
-      <c r="G19">
-        <f t="shared" si="1"/>
+      <c r="I19">
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="H19" t="str">
-        <f t="shared" si="2"/>
+      <c r="J19" t="str">
+        <f t="shared" si="3"/>
         <v>[18] = {</v>
       </c>
-      <c r="I19" t="str">
-        <f t="shared" si="3"/>
+      <c r="K19" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">["ID"] = 1879478542; </v>
       </c>
-      <c r="J19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K19" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
-      </c>
       <c r="L19" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">[19] = {}; -- </v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D20">
+        <v>304</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>[19] = {["CAT_ID"] = 304; }; -- Umbar-môkh</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="H20" t="str">
-        <f t="shared" si="2"/>
+      <c r="J20" t="str">
+        <f t="shared" si="3"/>
         <v>[19] = {</v>
       </c>
-      <c r="I20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="K20" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">[20] = {}; -- </v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">["CAT_ID"] = 304; </v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1879486409</v>
+      </c>
+      <c r="B21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
+        <v>[20] = {["ID"] = 1879486409; }; -- Light in the Umbar-môkh</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="H21" t="str">
-        <f t="shared" si="2"/>
+      <c r="J21" t="str">
+        <f t="shared" si="3"/>
         <v>[20] = {</v>
       </c>
-      <c r="I21" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="J21" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="K21" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486409; </v>
       </c>
       <c r="L21" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">[21] = {}; -- </v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1879486401</v>
+      </c>
+      <c r="B22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="1"/>
+        <v>[21] = {["ID"] = 1879486401; }; -- Slayer of the Umbar-môkh</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="H22" t="str">
-        <f t="shared" si="2"/>
+      <c r="J22" t="str">
+        <f t="shared" si="3"/>
         <v>[21] = {</v>
       </c>
-      <c r="I22" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="J22" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="K22" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486401; </v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">[22] = {}; -- </v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1879486271</v>
+      </c>
+      <c r="B23" t="s">
+        <v>190</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="1"/>
+        <v>[22] = {["ID"] = 1879486271; }; -- Slayer of Khabârkhad</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="H23" t="str">
-        <f t="shared" si="2"/>
+      <c r="J23" t="str">
+        <f t="shared" si="3"/>
         <v>[22] = {</v>
       </c>
-      <c r="I23" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="J23" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="K23" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486271; </v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F24" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">[23] = {}; -- </v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1879486272</v>
+      </c>
+      <c r="B24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>195</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="1"/>
+        <v>[23] = {["ID"] = 1879486272; }; -- Crypt-raider Slayer of Khabârkhad (Advanced)</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="H24" t="str">
-        <f t="shared" si="2"/>
+      <c r="J24" t="str">
+        <f t="shared" si="3"/>
         <v>[23] = {</v>
       </c>
-      <c r="I24" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="J24" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="K24" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486272; </v>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F25" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">[24] = {}; -- </v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1879486268</v>
+      </c>
+      <c r="B25" t="s">
+        <v>192</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>194</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v>[24] = {["ID"] = 1879486268; }; -- Crypt-raider Slayer of Khabârkhad</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="H25" t="str">
-        <f t="shared" si="2"/>
+      <c r="J25" t="str">
+        <f t="shared" si="3"/>
         <v>[24] = {</v>
       </c>
-      <c r="I25" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="J25" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="K25" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486268; </v>
       </c>
       <c r="L25" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F26" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">[25] = {}; -- </v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1879486252</v>
+      </c>
+      <c r="B26" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>197</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="1"/>
+        <v>[25] = {["ID"] = 1879486252; }; -- Spider-bane of Khabârkhad (Advanced)</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H26" t="str">
-        <f t="shared" si="2"/>
+      <c r="J26" t="str">
+        <f t="shared" si="3"/>
         <v>[25] = {</v>
       </c>
-      <c r="I26" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="J26" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="K26" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486252; </v>
       </c>
       <c r="L26" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F27" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">[26] = {}; -- </v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1879486253</v>
+      </c>
+      <c r="B27" t="s">
+        <v>198</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>199</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="1"/>
+        <v>[26] = {["ID"] = 1879486253; }; -- Spider-bane of Khabârkhad</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="H27" t="str">
-        <f t="shared" si="2"/>
+      <c r="J27" t="str">
+        <f t="shared" si="3"/>
         <v>[26] = {</v>
       </c>
-      <c r="I27" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="J27" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="K27" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486253; </v>
       </c>
       <c r="L27" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1879486270</v>
+      </c>
+      <c r="B28" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>203</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="H28" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  [] = {</v>
-      </c>
-      <c r="I28" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>[27] = {["ID"] = 1879486270; }; -- Dead-slayer of Khabârkhad (Advanced)</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" si="3"/>
+        <v>[27] = {</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486270; </v>
       </c>
       <c r="L28" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1879486269</v>
+      </c>
+      <c r="B29" t="s">
+        <v>201</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>202</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="H29" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  [] = {</v>
-      </c>
-      <c r="I29" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>[28] = {["ID"] = 1879486269; }; -- Dead-slayer of Khabârkhad</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>28</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" si="3"/>
+        <v>[28] = {</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486269; </v>
       </c>
       <c r="L29" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1879486280</v>
+      </c>
+      <c r="B30" t="s">
+        <v>204</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="H30" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  [] = {</v>
-      </c>
-      <c r="I30" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>[29] = {["ID"] = 1879486280; }; -- Slayer of Ilmabiri</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" si="3"/>
+        <v>[29] = {</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486280; </v>
       </c>
       <c r="L30" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1879486283</v>
+      </c>
+      <c r="B31" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>208</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="H31" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  [] = {</v>
-      </c>
-      <c r="I31" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>[30] = {["ID"] = 1879486283; }; -- Forsaken-slayer of Ilmabiri (Advanced)</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" si="3"/>
+        <v>[30] = {</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486283; </v>
       </c>
       <c r="L31" t="str">
-        <f t="shared" si="6"/>
-        <v>};</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1879486282</v>
+      </c>
+      <c r="B32" t="s">
+        <v>206</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>207</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="H32" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">  [] = {</v>
-      </c>
-      <c r="I32" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f t="shared" si="1"/>
+        <v>[31] = {["ID"] = 1879486282; }; -- Forsaken-slayer of Ilmabiri</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" si="3"/>
+        <v>[31] = {</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486282; </v>
       </c>
       <c r="L32" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1879486285</v>
+      </c>
+      <c r="B33" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>212</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="1"/>
+        <v>[32] = {["ID"] = 1879486285; }; -- Goblin-slayer of Ilmabiri (Advanced)</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="3"/>
+        <v>[32] = {</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486285; </v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1879486279</v>
+      </c>
+      <c r="B34" t="s">
+        <v>210</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>211</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="1"/>
+        <v>[33] = {["ID"] = 1879486279; }; -- Goblin-slayer of Ilmabiri</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="3"/>
+        <v>[33] = {</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486279; </v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1879486281</v>
+      </c>
+      <c r="B35" t="s">
+        <v>213</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>216</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="1"/>
+        <v>[34] = {["ID"] = 1879486281; }; -- Crocodile-slayer of Ilmabiri (Advanced)</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="3"/>
+        <v>[34] = {</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486281; </v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N35" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1879486284</v>
+      </c>
+      <c r="B36" t="s">
+        <v>214</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>215</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="1"/>
+        <v>[35] = {["ID"] = 1879486284; }; -- Crocodile-slayer of Ilmabiri</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="3"/>
+        <v>[35] = {</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486284; </v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1879486287</v>
+      </c>
+      <c r="B37" t="s">
+        <v>217</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="1"/>
+        <v>[36] = {["ID"] = 1879486287; }; -- Slayer of Kamrabezûr</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="3"/>
+        <v>[36] = {</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486287; </v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N37" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1879486292</v>
+      </c>
+      <c r="B38" t="s">
+        <v>218</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>221</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="1"/>
+        <v>[37] = {["ID"] = 1879486292; }; -- Cultist-slayer of Kamrabezûr (Advanced)</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="3"/>
+        <v>[37] = {</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486292; </v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N38" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1879486286</v>
+      </c>
+      <c r="B39" t="s">
+        <v>219</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>220</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="1"/>
+        <v>[38] = {["ID"] = 1879486286; }; -- Cultist-slayer of Kamrabezûr</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="3"/>
+        <v>[38] = {</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486286; </v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N39" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1879486289</v>
+      </c>
+      <c r="B40" t="s">
+        <v>222</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>225</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="1"/>
+        <v>[39] = {["ID"] = 1879486289; }; -- Gladiator-slayer of Kamrabezûr (Advanced)</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="3"/>
+        <v>[39] = {</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486289; </v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N40" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1879486291</v>
+      </c>
+      <c r="B41" t="s">
+        <v>223</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>224</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="1"/>
+        <v>[40] = {["ID"] = 1879486291; }; -- Gladiator-slayer of Kamrabezûr</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="3"/>
+        <v>[40] = {</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486291; </v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M41" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N41" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1879486290</v>
+      </c>
+      <c r="B42" t="s">
+        <v>226</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>229</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="1"/>
+        <v>[41] = {["ID"] = 1879486290; }; -- Dead-slayer of Kamrabezûr (Advanced)</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="3"/>
+        <v>[41] = {</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486290; </v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M42" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N42" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1879486288</v>
+      </c>
+      <c r="B43" t="s">
+        <v>227</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>228</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="1"/>
+        <v>[42] = {["ID"] = 1879486288; }; -- Dead-slayer of Kamrabezûr</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="3"/>
+        <v>[42] = {</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486288; </v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M43" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N43" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1879486295</v>
+      </c>
+      <c r="B44" t="s">
+        <v>230</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="1"/>
+        <v>[43] = {["ID"] = 1879486295; }; -- Slayer of Tâkhdar</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="3"/>
+        <v>[43] = {</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486295; </v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M44" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N44" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1879486296</v>
+      </c>
+      <c r="B45" t="s">
+        <v>231</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>234</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="1"/>
+        <v>[44] = {["ID"] = 1879486296; }; -- Grodbog-slayer of Tâkhdar (Advanced)</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="3"/>
+        <v>[44] = {</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486296; </v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M45" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N45" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1879486294</v>
+      </c>
+      <c r="B46" t="s">
+        <v>232</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>233</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="1"/>
+        <v>[45] = {["ID"] = 1879486294; }; -- Grodbog-slayer of Tâkhdar</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="3"/>
+        <v>[45] = {</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486294; </v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M46" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N46" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1879486293</v>
+      </c>
+      <c r="B47" t="s">
+        <v>235</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>238</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="1"/>
+        <v>[46] = {["ID"] = 1879486293; }; -- Smuggler-bane of Tâkhdar (Advanced)</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="3"/>
+        <v>[46] = {</v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486293; </v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M47" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N47" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1879486297</v>
+      </c>
+      <c r="B48" t="s">
+        <v>236</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>237</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="1"/>
+        <v>[47] = {["ID"] = 1879486297; }; -- Smuggler-bane of Tâkhdar</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="3"/>
+        <v>[47] = {</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486297; </v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M48" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N48" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1879486298</v>
+      </c>
+      <c r="B49" t="s">
+        <v>239</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>241</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="1"/>
+        <v>[48] = {["ID"] = 1879486298; }; -- Spider-bane of Tâkhdar (Advanced)</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="3"/>
+        <v>[48] = {</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486298; </v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M49" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N49" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1879486299</v>
+      </c>
+      <c r="B50" t="s">
+        <v>242</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>240</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="1"/>
+        <v>[49] = {["ID"] = 1879486299; }; -- Spider-bane of Tâkhdar</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="3"/>
+        <v>[49] = {</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486299; </v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M50" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N50" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1879486390</v>
+      </c>
+      <c r="B51" t="s">
+        <v>243</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" si="1"/>
+        <v>[50] = {["ID"] = 1879486390; }; -- Slayer of Dil-irmíz</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="3"/>
+        <v>[50] = {</v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486390; </v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M51" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N51" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1879486392</v>
+      </c>
+      <c r="B52" t="s">
+        <v>244</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>247</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="1"/>
+        <v>[51] = {["ID"] = 1879486392; }; -- Smuggler-bane of Dil-irmíz (Advanced)</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="3"/>
+        <v>[51] = {</v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486392; </v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M52" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N52" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1879486402</v>
+      </c>
+      <c r="B53" t="s">
+        <v>245</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>246</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="1"/>
+        <v>[52] = {["ID"] = 1879486402; }; -- Smuggler-bane of Dil-irmíz</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="3"/>
+        <v>[52] = {</v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486402; </v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M53" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N53" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1879486393</v>
+      </c>
+      <c r="B54" t="s">
+        <v>248</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>251</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="1"/>
+        <v>[53] = {["ID"] = 1879486393; }; -- Criminal-bane of Dil-irmíz (Advanced)</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="3"/>
+        <v>[53] = {</v>
+      </c>
+      <c r="K54" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486393; </v>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M54" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N54" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1879486403</v>
+      </c>
+      <c r="B55" t="s">
+        <v>249</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0</v>
+      </c>
+      <c r="E55" t="s">
+        <v>250</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="1"/>
+        <v>[54] = {["ID"] = 1879486403; }; -- Criminal-bane of Dil-irmíz</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="3"/>
+        <v>[54] = {</v>
+      </c>
+      <c r="K55" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486403; </v>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M55" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N55" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1879486404</v>
+      </c>
+      <c r="B56" t="s">
+        <v>253</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="1"/>
+        <v>[55] = {["ID"] = 1879486404; }; -- Explorer of the Umbar-môkh</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="J56" t="str">
+        <f t="shared" si="3"/>
+        <v>[55] = {</v>
+      </c>
+      <c r="K56" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486404; </v>
+      </c>
+      <c r="L56" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M56" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N56" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1879486395</v>
+      </c>
+      <c r="B57" t="s">
+        <v>254</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="1"/>
+        <v>[56] = {["ID"] = 1879486395; }; -- Reclaiming Khabârkhad</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="J57" t="str">
+        <f t="shared" si="3"/>
+        <v>[56] = {</v>
+      </c>
+      <c r="K57" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486395; </v>
+      </c>
+      <c r="L57" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M57" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N57" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1879486399</v>
+      </c>
+      <c r="B58" t="s">
+        <v>255</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="1"/>
+        <v>[57] = {["ID"] = 1879486399; }; -- Reclaiming Ilmabiri</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="J58" t="str">
+        <f t="shared" si="3"/>
+        <v>[57] = {</v>
+      </c>
+      <c r="K58" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486399; </v>
+      </c>
+      <c r="L58" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M58" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N58" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1879486400</v>
+      </c>
+      <c r="B59" t="s">
+        <v>256</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="1"/>
+        <v>[58] = {["ID"] = 1879486400; }; -- Reclaiming Kamrabezûr</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" si="3"/>
+        <v>[58] = {</v>
+      </c>
+      <c r="K59" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486400; </v>
+      </c>
+      <c r="L59" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M59" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N59" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1879486397</v>
+      </c>
+      <c r="B60" t="s">
+        <v>257</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="1"/>
+        <v>[59] = {["ID"] = 1879486397; }; -- Reclaiming Tâkhdar</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="J60" t="str">
+        <f t="shared" si="3"/>
+        <v>[59] = {</v>
+      </c>
+      <c r="K60" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486397; </v>
+      </c>
+      <c r="L60" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M60" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N60" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1879486391</v>
+      </c>
+      <c r="B61" t="s">
+        <v>258</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="1"/>
+        <v>[60] = {["ID"] = 1879486391; }; -- Reclaiming Dil-irmíz</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" si="3"/>
+        <v>[60] = {</v>
+      </c>
+      <c r="K61" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486391; </v>
+      </c>
+      <c r="L61" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M61" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N61" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1879486411</v>
+      </c>
+      <c r="B62" t="s">
+        <v>259</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="1"/>
+        <v>[61] = {["ID"] = 1879486411; }; -- Tales of the Umbar-môkh</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="J62" t="str">
+        <f t="shared" si="3"/>
+        <v>[61] = {</v>
+      </c>
+      <c r="K62" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486411; </v>
+      </c>
+      <c r="L62" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M62" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N62" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1879486408</v>
+      </c>
+      <c r="B63" t="s">
+        <v>260</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="1"/>
+        <v>[62] = {["ID"] = 1879486408; }; -- Tales of Khabârkhad</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" si="3"/>
+        <v>[62] = {</v>
+      </c>
+      <c r="K63" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486408; </v>
+      </c>
+      <c r="L63" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M63" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N63" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1879486410</v>
+      </c>
+      <c r="B64" t="s">
+        <v>261</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="1"/>
+        <v>[63] = {["ID"] = 1879486410; }; -- Tales of Ilmabiri</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="J64" t="str">
+        <f t="shared" si="3"/>
+        <v>[63] = {</v>
+      </c>
+      <c r="K64" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486410; </v>
+      </c>
+      <c r="L64" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M64" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N64" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1879486407</v>
+      </c>
+      <c r="B65" t="s">
+        <v>262</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="1"/>
+        <v>[64] = {["ID"] = 1879486407; }; -- Tales of Kamrabezûr</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" si="3"/>
+        <v>[64] = {</v>
+      </c>
+      <c r="K65" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486407; </v>
+      </c>
+      <c r="L65" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M65" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N65" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1879486412</v>
+      </c>
+      <c r="B66" t="s">
+        <v>263</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="1"/>
+        <v>[65] = {["ID"] = 1879486412; }; -- Tales of Tâkhdar</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" si="3"/>
+        <v>[65] = {</v>
+      </c>
+      <c r="K66" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">["ID"] = 1879486412; </v>
+      </c>
+      <c r="L66" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M66" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N66" t="str">
+        <f t="shared" si="7"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1879486406</v>
+      </c>
+      <c r="B67" t="s">
+        <v>264</v>
+      </c>
+      <c r="C67" s="1">
+        <v>0</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" ref="G67:G78" si="8">IF(AND(A67&gt;0,C67&gt;0),CONCATENATE("[",A67,"] = ",C67,", // ",B67),"")</f>
+        <v/>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" ref="H67:H78" si="9">CONCATENATE(J67,K67,L67,N67," -- ",B67)</f>
+        <v>[66] = {["ID"] = 1879486406; }; -- Tales of Dil-irmíz</v>
+      </c>
+      <c r="I67">
+        <f t="shared" ref="I67:I78" si="10">ROW()-1</f>
+        <v>66</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" ref="J67:J78" si="11">CONCATENATE(REPT(" ",2-LEN(I67)),"[",I67,"] = {")</f>
+        <v>[66] = {</v>
+      </c>
+      <c r="K67" t="str">
+        <f t="shared" ref="K67:K78" si="12">IF(LEN(A67)&gt;0,CONCATENATE("[""ID""] = ",A67,"; "),"")</f>
+        <v xml:space="preserve">["ID"] = 1879486406; </v>
+      </c>
+      <c r="L67" t="str">
+        <f t="shared" ref="L67:L78" si="13">IF(LEN(D67)&gt;0,CONCATENATE("[""CAT_ID""] = ",D67,"; "),"")</f>
+        <v/>
+      </c>
+      <c r="M67" t="str">
+        <f t="shared" ref="M67:M78" si="14">CONCATENATE("[""TIER""] = ",TEXT(C67,"0"),"; ")</f>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N67" t="str">
+        <f t="shared" ref="N67:N78" si="15">CONCATENATE("};")</f>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1879486405</v>
+      </c>
+      <c r="B68" t="s">
+        <v>265</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" si="9"/>
+        <v>[67] = {["ID"] = 1879486405; }; -- Vanquisher of Dil-irmíz</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="10"/>
+        <v>67</v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" si="11"/>
+        <v>[67] = {</v>
+      </c>
+      <c r="K68" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">["ID"] = 1879486405; </v>
+      </c>
+      <c r="L68" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="M68" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N68" t="str">
+        <f t="shared" si="15"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1879486396</v>
+      </c>
+      <c r="B69" t="s">
+        <v>266</v>
+      </c>
+      <c r="C69" s="1">
+        <v>0</v>
+      </c>
+      <c r="E69" t="s">
+        <v>267</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="9"/>
+        <v>[68] = {["ID"] = 1879486396; }; -- Cultist-bane of Dil-irmíz (Advanced)</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="10"/>
+        <v>68</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="11"/>
+        <v>[68] = {</v>
+      </c>
+      <c r="K69" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">["ID"] = 1879486396; </v>
+      </c>
+      <c r="L69" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="M69" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N69" t="str">
+        <f t="shared" si="15"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1879486394</v>
+      </c>
+      <c r="B70" t="s">
+        <v>268</v>
+      </c>
+      <c r="C70" s="1">
+        <v>0</v>
+      </c>
+      <c r="E70" t="s">
+        <v>269</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="H70" t="str">
+        <f t="shared" si="9"/>
+        <v>[69] = {["ID"] = 1879486394; }; -- Cultist-bane of Dil-irmíz</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="10"/>
+        <v>69</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" si="11"/>
+        <v>[69] = {</v>
+      </c>
+      <c r="K70" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">["ID"] = 1879486394; </v>
+      </c>
+      <c r="L70" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="M70" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N70" t="str">
+        <f t="shared" si="15"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1879486389</v>
+      </c>
+      <c r="B71" t="s">
+        <v>270</v>
+      </c>
+      <c r="C71" s="1">
+        <v>0</v>
+      </c>
+      <c r="E71" t="s">
+        <v>273</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="H71" t="str">
+        <f t="shared" si="9"/>
+        <v>[70] = {["ID"] = 1879486389; }; -- Darkwater-slayer of Dil-irmíz (Advanced)</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="10"/>
+        <v>70</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="11"/>
+        <v>[70] = {</v>
+      </c>
+      <c r="K71" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">["ID"] = 1879486389; </v>
+      </c>
+      <c r="L71" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="M71" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N71" t="str">
+        <f t="shared" si="15"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1879486398</v>
+      </c>
+      <c r="B72" t="s">
+        <v>271</v>
+      </c>
+      <c r="C72" s="1">
+        <v>0</v>
+      </c>
+      <c r="E72" t="s">
+        <v>272</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="H72" t="str">
+        <f t="shared" si="9"/>
+        <v>[71] = {["ID"] = 1879486398; }; -- Darkwater-slayer of Dil-irmíz</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="10"/>
+        <v>71</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" si="11"/>
+        <v>[71] = {</v>
+      </c>
+      <c r="K72" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">["ID"] = 1879486398; </v>
+      </c>
+      <c r="L72" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="M72" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N72" t="str">
+        <f t="shared" si="15"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1879486550</v>
+      </c>
+      <c r="B73" t="s">
+        <v>274</v>
+      </c>
+      <c r="C73" s="1">
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>277</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="H73" t="str">
+        <f t="shared" si="9"/>
+        <v>[72] = {["ID"] = 1879486550; }; -- Rat-slayer of the Umbar-môkh (Advanced)</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="10"/>
+        <v>72</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" si="11"/>
+        <v>[72] = {</v>
+      </c>
+      <c r="K73" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">["ID"] = 1879486550; </v>
+      </c>
+      <c r="L73" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="M73" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N73" t="str">
+        <f t="shared" si="15"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1879486551</v>
+      </c>
+      <c r="B74" t="s">
+        <v>275</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>276</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="H74" t="str">
+        <f t="shared" si="9"/>
+        <v>[73] = {["ID"] = 1879486551; }; -- Rat-slayer of the Umbar-môkh</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="10"/>
+        <v>73</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" si="11"/>
+        <v>[73] = {</v>
+      </c>
+      <c r="K74" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">["ID"] = 1879486551; </v>
+      </c>
+      <c r="L74" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="M74" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N74" t="str">
+        <f t="shared" si="15"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>1879486552</v>
+      </c>
+      <c r="B75" t="s">
+        <v>278</v>
+      </c>
+      <c r="C75" s="1">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>281</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="H75" t="str">
+        <f t="shared" si="9"/>
+        <v>[74] = {["ID"] = 1879486552; }; -- Bat-slayer of the Umbar-môkh (Advanced)</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="10"/>
+        <v>74</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" si="11"/>
+        <v>[74] = {</v>
+      </c>
+      <c r="K75" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">["ID"] = 1879486552; </v>
+      </c>
+      <c r="L75" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="M75" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N75" t="str">
+        <f t="shared" si="15"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1879486553</v>
+      </c>
+      <c r="B76" t="s">
+        <v>279</v>
+      </c>
+      <c r="C76" s="1">
+        <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>280</v>
+      </c>
+      <c r="G76" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="H76" t="str">
+        <f t="shared" si="9"/>
+        <v>[75] = {["ID"] = 1879486553; }; -- Bat-slayer of the Umbar-môkh</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="10"/>
+        <v>75</v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" si="11"/>
+        <v>[75] = {</v>
+      </c>
+      <c r="K76" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">["ID"] = 1879486553; </v>
+      </c>
+      <c r="L76" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="M76" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N76" t="str">
+        <f t="shared" si="15"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1879486571</v>
+      </c>
+      <c r="B77" t="s">
+        <v>282</v>
+      </c>
+      <c r="C77" s="1">
+        <v>0</v>
+      </c>
+      <c r="G77" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="H77" t="str">
+        <f t="shared" si="9"/>
+        <v>[76] = {["ID"] = 1879486571; }; -- Treasure-seeker of the Umbar-môkh</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="10"/>
+        <v>76</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="11"/>
+        <v>[76] = {</v>
+      </c>
+      <c r="K77" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">["ID"] = 1879486571; </v>
+      </c>
+      <c r="L77" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="M77" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N77" t="str">
+        <f t="shared" si="15"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G78" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="H78" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">[77] = {}; -- </v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="10"/>
+        <v>77</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="11"/>
+        <v>[77] = {</v>
+      </c>
+      <c r="K78" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="L78" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="M78" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N78" t="str">
+        <f t="shared" si="15"/>
         <v>};</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved Brine-belly to correct tab
</commit_message>
<xml_diff>
--- a/SourceFiles/DeedInfo-10-Haradwaith.xlsx
+++ b/SourceFiles/DeedInfo-10-Haradwaith.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkckx\Documents\The Lord of the Rings Online\Plugins\CubePlugins\DeedTracker\SourceFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B126BDF-C106-4370-9437-8771C1B696FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BB4184-6E39-49F0-82CE-62C60FE4AD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="869" activeTab="7" xr2:uid="{CDC9C16A-58F0-4807-B5CD-F77FF9D2EA43}"/>
+    <workbookView xWindow="4575" yWindow="0" windowWidth="22770" windowHeight="15600" tabRatio="869" activeTab="7" xr2:uid="{CDC9C16A-58F0-4807-B5CD-F77FF9D2EA43}"/>
   </bookViews>
   <sheets>
     <sheet name="Type" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="284">
   <si>
     <t>TIER</t>
   </si>
@@ -890,6 +890,9 @@
   </si>
   <si>
     <t>Treasure-seeker of the Umbar-môkh</t>
+  </si>
+  <si>
+    <t>Brine-belly</t>
   </si>
 </sst>
 </file>
@@ -4591,13 +4594,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E20F2D1-5B1C-4EE5-AF25-70FDE67F21F0}">
-  <dimension ref="A1:N78"/>
+  <dimension ref="A1:N79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B85" sqref="B85"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5515,11 +5518,11 @@
         <v>189</v>
       </c>
       <c r="C22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486401] = 1, // Slayer of the Umbar-môkh</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="1"/>
@@ -5543,7 +5546,7 @@
       </c>
       <c r="M22" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 1; </v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="7"/>
@@ -5558,11 +5561,11 @@
         <v>190</v>
       </c>
       <c r="C23" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486271] = 2, // Slayer of Khabârkhad</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="1"/>
@@ -5586,7 +5589,7 @@
       </c>
       <c r="M23" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="7"/>
@@ -5601,14 +5604,14 @@
         <v>191</v>
       </c>
       <c r="C24" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E24" t="s">
         <v>195</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486272] = 3, // Crypt-raider Slayer of Khabârkhad (Advanced)</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="1"/>
@@ -5632,7 +5635,7 @@
       </c>
       <c r="M24" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="7"/>
@@ -5647,14 +5650,14 @@
         <v>192</v>
       </c>
       <c r="C25" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E25" t="s">
         <v>194</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486268] = 4, // Crypt-raider Slayer of Khabârkhad</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="1"/>
@@ -5678,7 +5681,7 @@
       </c>
       <c r="M25" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="7"/>
@@ -5693,14 +5696,14 @@
         <v>196</v>
       </c>
       <c r="C26" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
         <v>197</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486252] = 3, // Spider-bane of Khabârkhad (Advanced)</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="1"/>
@@ -5724,7 +5727,7 @@
       </c>
       <c r="M26" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="7"/>
@@ -5739,14 +5742,14 @@
         <v>198</v>
       </c>
       <c r="C27" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E27" t="s">
         <v>199</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486253] = 4, // Spider-bane of Khabârkhad</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="1"/>
@@ -5770,7 +5773,7 @@
       </c>
       <c r="M27" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="7"/>
@@ -5785,14 +5788,14 @@
         <v>200</v>
       </c>
       <c r="C28" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E28" t="s">
         <v>203</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486270] = 3, // Dead-slayer of Khabârkhad (Advanced)</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="1"/>
@@ -5816,7 +5819,7 @@
       </c>
       <c r="M28" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="7"/>
@@ -5831,14 +5834,14 @@
         <v>201</v>
       </c>
       <c r="C29" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E29" t="s">
         <v>202</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486269] = 4, // Dead-slayer of Khabârkhad</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
@@ -5862,7 +5865,7 @@
       </c>
       <c r="M29" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="7"/>
@@ -5877,11 +5880,11 @@
         <v>204</v>
       </c>
       <c r="C30" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486280] = 2, // Slayer of Ilmabiri</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>
@@ -5905,7 +5908,7 @@
       </c>
       <c r="M30" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N30" t="str">
         <f t="shared" si="7"/>
@@ -5920,14 +5923,14 @@
         <v>205</v>
       </c>
       <c r="C31" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E31" t="s">
         <v>208</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486283] = 3, // Forsaken-slayer of Ilmabiri (Advanced)</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="1"/>
@@ -5951,7 +5954,7 @@
       </c>
       <c r="M31" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N31" t="str">
         <f t="shared" si="7"/>
@@ -5966,14 +5969,14 @@
         <v>206</v>
       </c>
       <c r="C32" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E32" t="s">
         <v>207</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486282] = 4, // Forsaken-slayer of Ilmabiri</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="1"/>
@@ -5997,7 +6000,7 @@
       </c>
       <c r="M32" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="7"/>
@@ -6012,14 +6015,14 @@
         <v>209</v>
       </c>
       <c r="C33" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E33" t="s">
         <v>212</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486285] = 3, // Goblin-slayer of Ilmabiri (Advanced)</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="1"/>
@@ -6043,7 +6046,7 @@
       </c>
       <c r="M33" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="7"/>
@@ -6058,14 +6061,14 @@
         <v>210</v>
       </c>
       <c r="C34" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E34" t="s">
         <v>211</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486279] = 4, // Goblin-slayer of Ilmabiri</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="1"/>
@@ -6089,7 +6092,7 @@
       </c>
       <c r="M34" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N34" t="str">
         <f t="shared" si="7"/>
@@ -6104,14 +6107,14 @@
         <v>213</v>
       </c>
       <c r="C35" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E35" t="s">
         <v>216</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486281] = 3, // Crocodile-slayer of Ilmabiri (Advanced)</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="1"/>
@@ -6135,7 +6138,7 @@
       </c>
       <c r="M35" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N35" t="str">
         <f t="shared" si="7"/>
@@ -6150,14 +6153,14 @@
         <v>214</v>
       </c>
       <c r="C36" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E36" t="s">
         <v>215</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486284] = 4, // Crocodile-slayer of Ilmabiri</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="1"/>
@@ -6181,7 +6184,7 @@
       </c>
       <c r="M36" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N36" t="str">
         <f t="shared" si="7"/>
@@ -6196,11 +6199,11 @@
         <v>217</v>
       </c>
       <c r="C37" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486287] = 2, // Slayer of Kamrabezûr</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="1"/>
@@ -6224,7 +6227,7 @@
       </c>
       <c r="M37" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N37" t="str">
         <f t="shared" si="7"/>
@@ -6239,14 +6242,14 @@
         <v>218</v>
       </c>
       <c r="C38" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E38" t="s">
         <v>221</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486292] = 3, // Cultist-slayer of Kamrabezûr (Advanced)</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="1"/>
@@ -6270,7 +6273,7 @@
       </c>
       <c r="M38" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N38" t="str">
         <f t="shared" si="7"/>
@@ -6285,14 +6288,14 @@
         <v>219</v>
       </c>
       <c r="C39" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E39" t="s">
         <v>220</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486286] = 4, // Cultist-slayer of Kamrabezûr</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="1"/>
@@ -6316,7 +6319,7 @@
       </c>
       <c r="M39" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N39" t="str">
         <f t="shared" si="7"/>
@@ -6331,14 +6334,14 @@
         <v>222</v>
       </c>
       <c r="C40" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E40" t="s">
         <v>225</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486289] = 3, // Gladiator-slayer of Kamrabezûr (Advanced)</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="1"/>
@@ -6362,7 +6365,7 @@
       </c>
       <c r="M40" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N40" t="str">
         <f t="shared" si="7"/>
@@ -6377,14 +6380,14 @@
         <v>223</v>
       </c>
       <c r="C41" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E41" t="s">
         <v>224</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486291] = 4, // Gladiator-slayer of Kamrabezûr</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="1"/>
@@ -6408,7 +6411,7 @@
       </c>
       <c r="M41" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N41" t="str">
         <f t="shared" si="7"/>
@@ -6423,14 +6426,14 @@
         <v>226</v>
       </c>
       <c r="C42" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E42" t="s">
         <v>229</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486290] = 3, // Dead-slayer of Kamrabezûr (Advanced)</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="1"/>
@@ -6454,7 +6457,7 @@
       </c>
       <c r="M42" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N42" t="str">
         <f t="shared" si="7"/>
@@ -6469,14 +6472,14 @@
         <v>227</v>
       </c>
       <c r="C43" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E43" t="s">
         <v>228</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486288] = 4, // Dead-slayer of Kamrabezûr</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="1"/>
@@ -6500,7 +6503,7 @@
       </c>
       <c r="M43" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N43" t="str">
         <f t="shared" si="7"/>
@@ -6515,11 +6518,11 @@
         <v>230</v>
       </c>
       <c r="C44" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486295] = 2, // Slayer of Tâkhdar</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="1"/>
@@ -6543,7 +6546,7 @@
       </c>
       <c r="M44" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N44" t="str">
         <f t="shared" si="7"/>
@@ -6558,14 +6561,14 @@
         <v>231</v>
       </c>
       <c r="C45" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E45" t="s">
         <v>234</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486296] = 3, // Grodbog-slayer of Tâkhdar (Advanced)</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="1"/>
@@ -6589,7 +6592,7 @@
       </c>
       <c r="M45" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N45" t="str">
         <f t="shared" si="7"/>
@@ -6604,14 +6607,14 @@
         <v>232</v>
       </c>
       <c r="C46" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E46" t="s">
         <v>233</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486294] = 4, // Grodbog-slayer of Tâkhdar</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="1"/>
@@ -6635,7 +6638,7 @@
       </c>
       <c r="M46" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N46" t="str">
         <f t="shared" si="7"/>
@@ -6650,14 +6653,14 @@
         <v>235</v>
       </c>
       <c r="C47" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E47" t="s">
         <v>238</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486293] = 3, // Smuggler-bane of Tâkhdar (Advanced)</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="1"/>
@@ -6681,7 +6684,7 @@
       </c>
       <c r="M47" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N47" t="str">
         <f t="shared" si="7"/>
@@ -6696,14 +6699,14 @@
         <v>236</v>
       </c>
       <c r="C48" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E48" t="s">
         <v>237</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486297] = 4, // Smuggler-bane of Tâkhdar</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="1"/>
@@ -6727,7 +6730,7 @@
       </c>
       <c r="M48" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N48" t="str">
         <f t="shared" si="7"/>
@@ -6742,14 +6745,14 @@
         <v>239</v>
       </c>
       <c r="C49" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E49" t="s">
         <v>241</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486298] = 3, // Spider-bane of Tâkhdar (Advanced)</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="1"/>
@@ -6773,7 +6776,7 @@
       </c>
       <c r="M49" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N49" t="str">
         <f t="shared" si="7"/>
@@ -6788,14 +6791,14 @@
         <v>242</v>
       </c>
       <c r="C50" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E50" t="s">
         <v>240</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486299] = 4, // Spider-bane of Tâkhdar</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="1"/>
@@ -6819,7 +6822,7 @@
       </c>
       <c r="M50" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N50" t="str">
         <f t="shared" si="7"/>
@@ -6834,11 +6837,11 @@
         <v>243</v>
       </c>
       <c r="C51" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486390] = 2, // Slayer of Dil-irmíz</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="1"/>
@@ -6862,7 +6865,7 @@
       </c>
       <c r="M51" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N51" t="str">
         <f t="shared" si="7"/>
@@ -6877,14 +6880,14 @@
         <v>244</v>
       </c>
       <c r="C52" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E52" t="s">
         <v>247</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486392] = 3, // Smuggler-bane of Dil-irmíz (Advanced)</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="1"/>
@@ -6908,7 +6911,7 @@
       </c>
       <c r="M52" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N52" t="str">
         <f t="shared" si="7"/>
@@ -6923,14 +6926,14 @@
         <v>245</v>
       </c>
       <c r="C53" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E53" t="s">
         <v>246</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486402] = 4, // Smuggler-bane of Dil-irmíz</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="1"/>
@@ -6954,7 +6957,7 @@
       </c>
       <c r="M53" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N53" t="str">
         <f t="shared" si="7"/>
@@ -6969,14 +6972,14 @@
         <v>248</v>
       </c>
       <c r="C54" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E54" t="s">
         <v>251</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486393] = 3, // Criminal-bane of Dil-irmíz (Advanced)</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="1"/>
@@ -7000,7 +7003,7 @@
       </c>
       <c r="M54" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 3; </v>
       </c>
       <c r="N54" t="str">
         <f t="shared" si="7"/>
@@ -7015,14 +7018,14 @@
         <v>249</v>
       </c>
       <c r="C55" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E55" t="s">
         <v>250</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486403] = 4, // Criminal-bane of Dil-irmíz</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="1"/>
@@ -7046,7 +7049,7 @@
       </c>
       <c r="M55" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 4; </v>
       </c>
       <c r="N55" t="str">
         <f t="shared" si="7"/>
@@ -7061,11 +7064,11 @@
         <v>253</v>
       </c>
       <c r="C56" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486404] = 1, // Explorer of the Umbar-môkh</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="1"/>
@@ -7089,7 +7092,7 @@
       </c>
       <c r="M56" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 1; </v>
       </c>
       <c r="N56" t="str">
         <f t="shared" si="7"/>
@@ -7104,11 +7107,11 @@
         <v>254</v>
       </c>
       <c r="C57" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486395] = 2, // Reclaiming Khabârkhad</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="1"/>
@@ -7132,7 +7135,7 @@
       </c>
       <c r="M57" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N57" t="str">
         <f t="shared" si="7"/>
@@ -7147,11 +7150,11 @@
         <v>255</v>
       </c>
       <c r="C58" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486399] = 2, // Reclaiming Ilmabiri</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="1"/>
@@ -7175,7 +7178,7 @@
       </c>
       <c r="M58" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N58" t="str">
         <f t="shared" si="7"/>
@@ -7190,11 +7193,11 @@
         <v>256</v>
       </c>
       <c r="C59" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486400] = 2, // Reclaiming Kamrabezûr</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="1"/>
@@ -7218,7 +7221,7 @@
       </c>
       <c r="M59" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N59" t="str">
         <f t="shared" si="7"/>
@@ -7233,11 +7236,11 @@
         <v>257</v>
       </c>
       <c r="C60" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486397] = 2, // Reclaiming Tâkhdar</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="1"/>
@@ -7261,7 +7264,7 @@
       </c>
       <c r="M60" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N60" t="str">
         <f t="shared" si="7"/>
@@ -7276,11 +7279,11 @@
         <v>258</v>
       </c>
       <c r="C61" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486391] = 2, // Reclaiming Dil-irmíz</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="1"/>
@@ -7304,7 +7307,7 @@
       </c>
       <c r="M61" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N61" t="str">
         <f t="shared" si="7"/>
@@ -7319,11 +7322,11 @@
         <v>259</v>
       </c>
       <c r="C62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486411] = 1, // Tales of the Umbar-môkh</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="1"/>
@@ -7347,7 +7350,7 @@
       </c>
       <c r="M62" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 1; </v>
       </c>
       <c r="N62" t="str">
         <f t="shared" si="7"/>
@@ -7362,11 +7365,11 @@
         <v>260</v>
       </c>
       <c r="C63" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486408] = 2, // Tales of Khabârkhad</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="1"/>
@@ -7390,7 +7393,7 @@
       </c>
       <c r="M63" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N63" t="str">
         <f t="shared" si="7"/>
@@ -7405,11 +7408,11 @@
         <v>261</v>
       </c>
       <c r="C64" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486410] = 2, // Tales of Ilmabiri</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="1"/>
@@ -7433,7 +7436,7 @@
       </c>
       <c r="M64" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N64" t="str">
         <f t="shared" si="7"/>
@@ -7448,11 +7451,11 @@
         <v>262</v>
       </c>
       <c r="C65" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486407] = 2, // Tales of Kamrabezûr</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="1"/>
@@ -7476,7 +7479,7 @@
       </c>
       <c r="M65" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N65" t="str">
         <f t="shared" si="7"/>
@@ -7491,11 +7494,11 @@
         <v>263</v>
       </c>
       <c r="C66" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>[1879486412] = 2, // Tales of Tâkhdar</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="1"/>
@@ -7519,7 +7522,7 @@
       </c>
       <c r="M66" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N66" t="str">
         <f t="shared" si="7"/>
@@ -7534,18 +7537,18 @@
         <v>264</v>
       </c>
       <c r="C67" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G67" t="str">
         <f t="shared" ref="G67:G78" si="8">IF(AND(A67&gt;0,C67&gt;0),CONCATENATE("[",A67,"] = ",C67,", // ",B67),"")</f>
-        <v/>
+        <v>[1879486406] = 2, // Tales of Dil-irmíz</v>
       </c>
       <c r="H67" t="str">
         <f t="shared" ref="H67:H78" si="9">CONCATENATE(J67,K67,L67,N67," -- ",B67)</f>
         <v>[66] = {["ID"] = 1879486406; }; -- Tales of Dil-irmíz</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I78" si="10">ROW()-1</f>
+        <f t="shared" ref="I67:I79" si="10">ROW()-1</f>
         <v>66</v>
       </c>
       <c r="J67" t="str">
@@ -7562,10 +7565,10 @@
       </c>
       <c r="M67" t="str">
         <f t="shared" ref="M67:M78" si="14">CONCATENATE("[""TIER""] = ",TEXT(C67,"0"),"; ")</f>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N67" t="str">
-        <f t="shared" ref="N67:N78" si="15">CONCATENATE("};")</f>
+        <f t="shared" ref="N67:N79" si="15">CONCATENATE("};")</f>
         <v>};</v>
       </c>
     </row>
@@ -7620,14 +7623,14 @@
         <v>266</v>
       </c>
       <c r="C69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" t="s">
         <v>267</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>[1879486396] = 1, // Cultist-bane of Dil-irmíz (Advanced)</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="9"/>
@@ -7651,7 +7654,7 @@
       </c>
       <c r="M69" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 1; </v>
       </c>
       <c r="N69" t="str">
         <f t="shared" si="15"/>
@@ -7666,14 +7669,14 @@
         <v>268</v>
       </c>
       <c r="C70" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E70" t="s">
         <v>269</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>[1879486394] = 2, // Cultist-bane of Dil-irmíz</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="9"/>
@@ -7697,7 +7700,7 @@
       </c>
       <c r="M70" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N70" t="str">
         <f t="shared" si="15"/>
@@ -7712,14 +7715,14 @@
         <v>270</v>
       </c>
       <c r="C71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" t="s">
         <v>273</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>[1879486389] = 1, // Darkwater-slayer of Dil-irmíz (Advanced)</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="9"/>
@@ -7743,7 +7746,7 @@
       </c>
       <c r="M71" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 1; </v>
       </c>
       <c r="N71" t="str">
         <f t="shared" si="15"/>
@@ -7758,14 +7761,14 @@
         <v>271</v>
       </c>
       <c r="C72" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E72" t="s">
         <v>272</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>[1879486398] = 2, // Darkwater-slayer of Dil-irmíz</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="9"/>
@@ -7789,7 +7792,7 @@
       </c>
       <c r="M72" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N72" t="str">
         <f t="shared" si="15"/>
@@ -7804,14 +7807,14 @@
         <v>274</v>
       </c>
       <c r="C73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E73" t="s">
         <v>277</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>[1879486550] = 1, // Rat-slayer of the Umbar-môkh (Advanced)</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="9"/>
@@ -7835,7 +7838,7 @@
       </c>
       <c r="M73" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 1; </v>
       </c>
       <c r="N73" t="str">
         <f t="shared" si="15"/>
@@ -7850,14 +7853,14 @@
         <v>275</v>
       </c>
       <c r="C74" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E74" t="s">
         <v>276</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>[1879486551] = 2, // Rat-slayer of the Umbar-môkh</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="9"/>
@@ -7881,7 +7884,7 @@
       </c>
       <c r="M74" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N74" t="str">
         <f t="shared" si="15"/>
@@ -7896,14 +7899,14 @@
         <v>278</v>
       </c>
       <c r="C75" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E75" t="s">
         <v>281</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>[1879486552] = 1, // Bat-slayer of the Umbar-môkh (Advanced)</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" si="9"/>
@@ -7927,7 +7930,7 @@
       </c>
       <c r="M75" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 1; </v>
       </c>
       <c r="N75" t="str">
         <f t="shared" si="15"/>
@@ -7942,14 +7945,14 @@
         <v>279</v>
       </c>
       <c r="C76" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E76" t="s">
         <v>280</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>[1879486553] = 2, // Bat-slayer of the Umbar-môkh</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="9"/>
@@ -7973,7 +7976,7 @@
       </c>
       <c r="M76" t="str">
         <f t="shared" si="14"/>
-        <v xml:space="preserve">["TIER"] = 0; </v>
+        <v xml:space="preserve">["TIER"] = 2; </v>
       </c>
       <c r="N76" t="str">
         <f t="shared" si="15"/>
@@ -7995,7 +7998,7 @@
         <v/>
       </c>
       <c r="H77" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="H77:H79" si="16">CONCATENATE(J77,K77,L77,N77," -- ",B77)</f>
         <v>[76] = {["ID"] = 1879486571; }; -- Treasure-seeker of the Umbar-môkh</v>
       </c>
       <c r="I77">
@@ -8003,19 +8006,19 @@
         <v>76</v>
       </c>
       <c r="J77" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="J77:J79" si="17">CONCATENATE(REPT(" ",2-LEN(I77)),"[",I77,"] = {")</f>
         <v>[76] = {</v>
       </c>
       <c r="K77" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="K77:K79" si="18">IF(LEN(A77)&gt;0,CONCATENATE("[""ID""] = ",A77,"; "),"")</f>
         <v xml:space="preserve">["ID"] = 1879486571; </v>
       </c>
       <c r="L77" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="L77:L79" si="19">IF(LEN(D77)&gt;0,CONCATENATE("[""CAT_ID""] = ",D77,"; "),"")</f>
         <v/>
       </c>
       <c r="M77" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="M77:M79" si="20">CONCATENATE("[""TIER""] = ",TEXT(C77,"0"),"; ")</f>
         <v xml:space="preserve">["TIER"] = 0; </v>
       </c>
       <c r="N77" t="str">
@@ -8024,35 +8027,74 @@
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1879485102</v>
+      </c>
+      <c r="B78" t="s">
+        <v>283</v>
+      </c>
+      <c r="C78" s="1">
+        <v>0</v>
+      </c>
       <c r="G78" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="H78" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">[77] = {}; -- </v>
+        <f t="shared" si="16"/>
+        <v>[77] = {["ID"] = 1879485102; }; -- Brine-belly</v>
       </c>
       <c r="I78">
         <f t="shared" si="10"/>
         <v>77</v>
       </c>
       <c r="J78" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>[77] = {</v>
       </c>
       <c r="K78" t="str">
-        <f t="shared" si="12"/>
-        <v/>
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">["ID"] = 1879485102; </v>
       </c>
       <c r="L78" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="M78" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">["TIER"] = 0; </v>
       </c>
       <c r="N78" t="str">
+        <f t="shared" si="15"/>
+        <v>};</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H79" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">[78] = {}; -- </v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="10"/>
+        <v>78</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="17"/>
+        <v>[78] = {</v>
+      </c>
+      <c r="K79" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="L79" t="str">
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+      <c r="M79" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">["TIER"] = 0; </v>
+      </c>
+      <c r="N79" t="str">
         <f t="shared" si="15"/>
         <v>};</v>
       </c>

</xml_diff>